<commit_message>
Fix serial issue Add initial Lowpower support Fix some example Add new example Update FreeRTOS library Add Lowpower example Remove doc file
</commit_message>
<xml_diff>
--- a/libraries/BoardExamples/examples/all_boards/Benchmarks/Benchmarks-results.xlsx
+++ b/libraries/BoardExamples/examples/all_boards/Benchmarks/Benchmarks-results.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="120" windowWidth="18225" windowHeight="10125"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="58">
   <si>
     <t>Board</t>
   </si>
@@ -178,14 +178,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>1.       Running in sram: SRAM split into code and date block. Built select "startup addr at sram" from the menu option</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">                tested by huaweiwx@sina.com 2018.7.2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>3.       Digital Toggle hard (Khz) use a frequency counter to get the "Digital Toggle" result</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -198,10 +190,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>2.       Digital Read &amp; Digital Write pin use LL lib but F7 use HAL</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>NUCLEO-F767</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -210,7 +198,23 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>Mega 2560</t>
+    <t>2.       Digital Read &amp; Digital Write pin use LL lib but H7 not</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>STM32F103</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">                tested by huaweiwx@sina.com 2018.7</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.       Running in sram: SRAM split into code and date block. Built  option  selected  "startup addr at sram" from the menu</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>4.       Arduino ide v1.8.5 for STM32GENERIC compliled with GCC ver 5.4.1-2016q2</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -218,6 +222,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="176" formatCode="#,##0_);[Red]\(#,##0\)"/>
+  </numFmts>
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -362,7 +369,7 @@
       <charset val="134"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -545,6 +552,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -856,7 +869,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -887,6 +900,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -904,15 +929,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1256,73 +1272,79 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R17"/>
+  <dimension ref="A1:S18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="Q26" sqref="Q26"/>
+      <selection pane="bottomRight" activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.875" customWidth="1"/>
-    <col min="2" max="4" width="8.75" customWidth="1"/>
-    <col min="5" max="5" width="8.625" customWidth="1"/>
-    <col min="6" max="6" width="8.75" customWidth="1"/>
-    <col min="7" max="7" width="8.625" customWidth="1"/>
-    <col min="8" max="8" width="7.875" customWidth="1"/>
-    <col min="9" max="9" width="7.125" customWidth="1"/>
-    <col min="10" max="10" width="7.875" customWidth="1"/>
-    <col min="11" max="12" width="10.25" customWidth="1"/>
-    <col min="13" max="14" width="8.75" customWidth="1"/>
-    <col min="15" max="16" width="8.625" customWidth="1"/>
-    <col min="17" max="17" width="9.5" customWidth="1"/>
-    <col min="18" max="18" width="12.5" customWidth="1"/>
+    <col min="1" max="1" width="21.375" customWidth="1"/>
+    <col min="2" max="2" width="8.75" customWidth="1"/>
+    <col min="3" max="3" width="9.875" customWidth="1"/>
+    <col min="4" max="4" width="8.875" customWidth="1"/>
+    <col min="5" max="6" width="8.625" customWidth="1"/>
+    <col min="7" max="7" width="8.125" customWidth="1"/>
+    <col min="8" max="8" width="9" customWidth="1"/>
+    <col min="9" max="9" width="8.25" customWidth="1"/>
+    <col min="10" max="10" width="8.625" customWidth="1"/>
+    <col min="11" max="11" width="7.75" customWidth="1"/>
+    <col min="12" max="12" width="8.375" customWidth="1"/>
+    <col min="13" max="13" width="7.125" customWidth="1"/>
+    <col min="14" max="14" width="8.625" customWidth="1"/>
+    <col min="15" max="15" width="8.75" customWidth="1"/>
+    <col min="16" max="16" width="7.875" customWidth="1"/>
+    <col min="17" max="17" width="7.5" customWidth="1"/>
+    <col min="18" max="18" width="7.75" customWidth="1"/>
+    <col min="19" max="19" width="6.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="1" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" s="1" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="C1" s="15"/>
-      <c r="D1" s="10" t="s">
+      <c r="C1" s="19"/>
+      <c r="D1" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1" s="15"/>
+      <c r="F1" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="G1" s="15"/>
+      <c r="H1" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="I1" s="15"/>
+      <c r="J1" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="K1" s="15"/>
+      <c r="L1" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="M1" s="17"/>
+      <c r="N1" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="O1" s="15"/>
+      <c r="P1" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="E1" s="11"/>
-      <c r="F1" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="G1" s="11"/>
-      <c r="H1" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="I1" s="11"/>
-      <c r="J1" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="K1" s="11"/>
-      <c r="L1" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="M1" s="13"/>
-      <c r="N1" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="O1" s="11"/>
-      <c r="P1" s="12" t="s">
+      <c r="Q1" s="17"/>
+      <c r="R1" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="Q1" s="13"/>
-      <c r="R1" s="5" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="S1" s="17"/>
+    </row>
+    <row r="2" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>36</v>
       </c>
@@ -1369,70 +1391,78 @@
         <v>168</v>
       </c>
       <c r="P2" s="2">
+        <v>72</v>
+      </c>
+      <c r="Q2" s="2">
+        <v>72</v>
+      </c>
+      <c r="R2" s="2">
         <v>120</v>
       </c>
-      <c r="Q2" s="2">
+      <c r="S2" s="2">
         <v>120</v>
       </c>
-      <c r="R2" s="17">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>35</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>34</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>34</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>34</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>34</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>34</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="M3" s="2" t="s">
         <v>34</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="O3" s="2" t="s">
         <v>34</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="Q3" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="R3" s="18"/>
-    </row>
-    <row r="4" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="R3" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -1450,9 +1480,10 @@
       <c r="O4" s="2"/>
       <c r="P4" s="2"/>
       <c r="Q4" s="2"/>
-      <c r="R4" s="18"/>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="R4" s="2"/>
+      <c r="S4" s="2"/>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>16</v>
       </c>
@@ -1462,9 +1493,15 @@
       <c r="C5" s="3">
         <v>390.62</v>
       </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
+      <c r="D5" s="3">
+        <v>208.77</v>
+      </c>
+      <c r="E5" s="3">
+        <v>160.26</v>
+      </c>
+      <c r="F5" s="3">
+        <v>133.69</v>
+      </c>
       <c r="G5" s="3">
         <v>106.16</v>
       </c>
@@ -1474,7 +1511,9 @@
       <c r="I5" s="3">
         <v>66.010000000000005</v>
       </c>
-      <c r="J5" s="3"/>
+      <c r="J5" s="3">
+        <v>65.45</v>
+      </c>
       <c r="K5" s="3">
         <v>51.44</v>
       </c>
@@ -1490,45 +1529,73 @@
       <c r="O5" s="3">
         <v>94.7</v>
       </c>
-      <c r="P5" s="3"/>
+      <c r="P5" s="3">
+        <v>7.4</v>
+      </c>
       <c r="Q5" s="3">
+        <v>7.41</v>
+      </c>
+      <c r="R5" s="3"/>
+      <c r="S5" s="3">
         <v>8.26</v>
       </c>
-      <c r="R5" s="18">
-        <v>6.15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4">
+      <c r="B6" s="4">
+        <v>1073979.6599999999</v>
+      </c>
+      <c r="C6" s="13">
+        <v>1073979.6599999999</v>
+      </c>
+      <c r="D6" s="13">
+        <v>575801.81000000006</v>
+      </c>
+      <c r="E6" s="13">
+        <v>236739.25</v>
+      </c>
+      <c r="F6" s="13">
+        <v>221864.28</v>
+      </c>
+      <c r="G6" s="12">
+        <v>160490.09</v>
+      </c>
+      <c r="H6" s="13">
         <v>147484.29</v>
       </c>
-      <c r="I6" s="4">
+      <c r="I6" s="13">
         <v>100325.89</v>
       </c>
-      <c r="J6" s="4"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="16">
+      <c r="J6" s="13">
+        <v>114669</v>
+      </c>
+      <c r="K6" s="12">
+        <v>88821.91</v>
+      </c>
+      <c r="L6" s="12">
         <v>103669.52</v>
       </c>
-      <c r="M6" s="4">
+      <c r="M6" s="13">
         <v>84938</v>
       </c>
-      <c r="N6" s="4"/>
-      <c r="O6" s="4"/>
-      <c r="P6" s="4"/>
-      <c r="Q6" s="4"/>
-      <c r="R6" s="18"/>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="N6" s="13">
+        <v>205808.6</v>
+      </c>
+      <c r="O6" s="13">
+        <v>142412.6</v>
+      </c>
+      <c r="P6" s="13">
+        <v>61112.83</v>
+      </c>
+      <c r="Q6" s="13">
+        <v>75633.94</v>
+      </c>
+      <c r="R6" s="4"/>
+      <c r="S6" s="4"/>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>33</v>
       </c>
@@ -1538,9 +1605,15 @@
       <c r="C7" s="3">
         <v>611.26</v>
       </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
+      <c r="D7" s="3">
+        <v>327.72</v>
+      </c>
+      <c r="E7" s="3">
+        <v>134.74</v>
+      </c>
+      <c r="F7" s="3">
+        <v>126.27</v>
+      </c>
       <c r="G7" s="3">
         <v>91.34</v>
       </c>
@@ -1550,7 +1623,9 @@
       <c r="I7" s="3">
         <v>57.1</v>
       </c>
-      <c r="J7" s="3"/>
+      <c r="J7" s="3">
+        <v>65.260000000000005</v>
+      </c>
       <c r="K7" s="3">
         <v>50.55</v>
       </c>
@@ -1566,15 +1641,18 @@
       <c r="O7" s="3">
         <v>81.05</v>
       </c>
-      <c r="P7" s="3"/>
+      <c r="P7" s="3">
+        <v>34.78</v>
+      </c>
       <c r="Q7" s="3">
+        <v>43.05</v>
+      </c>
+      <c r="R7" s="3"/>
+      <c r="S7" s="3">
         <v>50.14</v>
       </c>
-      <c r="R7" s="18">
-        <v>10.119999999999999</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A8" s="5"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -1592,101 +1670,120 @@
       <c r="O8" s="3"/>
       <c r="P8" s="3"/>
       <c r="Q8" s="3"/>
-      <c r="R8" s="18"/>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="R8" s="3"/>
+      <c r="S8" s="3"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="10">
         <v>25826.45</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="11">
         <v>25826.45</v>
       </c>
-      <c r="D9" s="3"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="16">
+      <c r="D9" s="12">
+        <v>39204.92</v>
+      </c>
+      <c r="E9" s="12">
+        <v>39183.42</v>
+      </c>
+      <c r="F9" s="12">
+        <v>35947</v>
+      </c>
+      <c r="G9" s="12">
         <v>29944.6</v>
       </c>
-      <c r="H9" s="3">
+      <c r="H9" s="12">
         <v>23946.36</v>
       </c>
-      <c r="I9" s="3">
+      <c r="I9" s="12">
         <v>23946.36</v>
       </c>
-      <c r="J9" s="3">
-        <v>14963</v>
-      </c>
-      <c r="K9" s="16">
+      <c r="J9" s="12">
+        <v>20959.53</v>
+      </c>
+      <c r="K9" s="12">
         <v>20945.919999999998</v>
       </c>
-      <c r="L9" s="16">
+      <c r="L9" s="12">
         <v>19952.91</v>
       </c>
-      <c r="M9" s="3">
+      <c r="M9" s="12">
         <v>19935</v>
       </c>
-      <c r="N9" s="3">
+      <c r="N9" s="12">
         <v>33550.29</v>
       </c>
-      <c r="O9" s="3">
+      <c r="O9" s="12">
         <v>20967</v>
       </c>
-      <c r="P9" s="3"/>
-      <c r="Q9" s="3"/>
-      <c r="R9" s="18">
-        <v>116.93</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="P9" s="12">
+        <v>10265.459999999999</v>
+      </c>
+      <c r="Q9" s="12">
+        <v>7188.5</v>
+      </c>
+      <c r="R9" s="3"/>
+      <c r="S9" s="3"/>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="10">
         <v>42163.85</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="11">
         <v>42163.85</v>
       </c>
-      <c r="D10" s="3"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="16">
+      <c r="D10" s="12">
+        <v>61606.7</v>
+      </c>
+      <c r="E10" s="12">
+        <v>20549.07</v>
+      </c>
+      <c r="F10" s="12">
+        <v>19984</v>
+      </c>
+      <c r="G10" s="12">
         <v>12845.71</v>
       </c>
-      <c r="H10" s="3">
+      <c r="H10" s="12">
         <v>17121.240000000002</v>
       </c>
-      <c r="I10" s="3">
-        <v>17121.240000000002</v>
-      </c>
-      <c r="J10" s="3">
+      <c r="I10" s="12">
+        <v>13984.06</v>
+      </c>
+      <c r="J10" s="12">
         <v>11979</v>
       </c>
-      <c r="K10" s="16">
+      <c r="K10" s="12">
         <v>10485.92</v>
       </c>
-      <c r="L10" s="16">
+      <c r="L10" s="12">
         <v>13316.29</v>
       </c>
-      <c r="M10" s="3">
+      <c r="M10" s="12">
         <v>9984</v>
       </c>
-      <c r="N10" s="3">
+      <c r="N10" s="12">
         <v>23977.37</v>
       </c>
-      <c r="O10" s="3">
+      <c r="O10" s="12">
         <v>10490</v>
       </c>
-      <c r="P10" s="3"/>
-      <c r="Q10" s="3"/>
-      <c r="R10" s="18">
-        <v>101.94</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="P10" s="12">
+        <v>11979.06</v>
+      </c>
+      <c r="Q10" s="12">
+        <v>5992.83</v>
+      </c>
+      <c r="R10" s="3"/>
+      <c r="S10" s="3"/>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>45</v>
       </c>
@@ -1706,43 +1803,50 @@
       <c r="O11" s="3"/>
       <c r="P11" s="3"/>
       <c r="Q11" s="3"/>
-      <c r="R11" s="18"/>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="R11" s="3"/>
+      <c r="S11" s="3"/>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
       <c r="C13" s="7" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
       <c r="C14" s="7" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
       <c r="C15" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
       <c r="C16" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C17" s="7" t="s">
-        <v>49</v>
+      <c r="C17" s="6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="18" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C18" s="7" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="9">
     <mergeCell ref="N1:O1"/>
-    <mergeCell ref="P1:Q1"/>
+    <mergeCell ref="R1:S1"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="H1:I1"/>
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="L1:M1"/>
     <mergeCell ref="D1:E1"/>
+    <mergeCell ref="P1:Q1"/>
   </mergeCells>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1755,7 +1859,7 @@
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1765,12 +1869,12 @@
     <col min="3" max="3" width="7.375" customWidth="1"/>
     <col min="4" max="4" width="8" customWidth="1"/>
     <col min="5" max="5" width="7.625" customWidth="1"/>
-    <col min="6" max="6" width="9.75" customWidth="1"/>
-    <col min="8" max="8" width="8.25" customWidth="1"/>
+    <col min="6" max="6" width="13.375" customWidth="1"/>
+    <col min="8" max="8" width="15.375" customWidth="1"/>
     <col min="9" max="9" width="9.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" ht="71.25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" s="1" customFormat="1" ht="57" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2408,14 +2512,14 @@
         <v>1615</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" ht="76.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="F23" t="s">
+      <c r="F23" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="H23" t="s">
+      <c r="H23" s="1" t="s">
         <v>47</v>
       </c>
     </row>

</xml_diff>

<commit_message>
merge from huaweiwx remove unused doc
</commit_message>
<xml_diff>
--- a/libraries/BoardExamples/examples/all_boards/Benchmarks/Benchmarks-results.xlsx
+++ b/libraries/BoardExamples/examples/all_boards/Benchmarks/Benchmarks-results.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="120" windowWidth="18225" windowHeight="10125"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="63">
   <si>
     <t>Board</t>
   </si>
@@ -231,6 +231,10 @@
   </si>
   <si>
     <t>EFM32G222F</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>NANO120</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -941,22 +945,22 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1303,13 +1307,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X18"/>
+  <dimension ref="A1:Y18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="X14" sqref="X14"/>
+      <selection pane="bottomRight" activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1337,16 +1341,17 @@
     <col min="22" max="22" width="7.375" customWidth="1"/>
     <col min="23" max="23" width="8.125" customWidth="1"/>
     <col min="24" max="24" width="7.5" customWidth="1"/>
+    <col min="25" max="25" width="9.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="1" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:25" s="1" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="C1" s="20"/>
+      <c r="C1" s="16"/>
       <c r="D1" s="17" t="s">
         <v>51</v>
       </c>
@@ -1371,27 +1376,30 @@
         <v>52</v>
       </c>
       <c r="O1" s="18"/>
-      <c r="P1" s="15" t="s">
+      <c r="P1" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="Q1" s="16"/>
+      <c r="Q1" s="20"/>
       <c r="R1" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="S1" s="15" t="s">
+      <c r="S1" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="T1" s="16"/>
-      <c r="U1" s="15" t="s">
+      <c r="T1" s="20"/>
+      <c r="U1" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="V1" s="16"/>
+      <c r="V1" s="20"/>
       <c r="W1" s="17" t="s">
         <v>61</v>
       </c>
       <c r="X1" s="21"/>
-    </row>
-    <row r="2" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Y1" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>36</v>
       </c>
@@ -1464,8 +1472,11 @@
       <c r="X2" s="2">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Y2" s="2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>35</v>
       </c>
@@ -1538,8 +1549,11 @@
       <c r="X3" s="2" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="4" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Y3" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5"/>
       <c r="B4" s="2" t="s">
         <v>58</v>
@@ -1576,8 +1590,9 @@
       <c r="V4" s="2"/>
       <c r="W4" s="2"/>
       <c r="X4" s="2"/>
-    </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="Y4" s="2"/>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>16</v>
       </c>
@@ -1644,8 +1659,9 @@
       </c>
       <c r="W5" s="3"/>
       <c r="X5" s="3"/>
-    </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="Y5" s="3"/>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>32</v>
       </c>
@@ -1714,8 +1730,11 @@
       <c r="X6" s="12">
         <v>25764</v>
       </c>
-    </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="Y6" s="12">
+        <v>36208</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>33</v>
       </c>
@@ -1786,8 +1805,11 @@
       <c r="X7" s="3">
         <v>14.66</v>
       </c>
-    </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="Y7" s="3">
+        <v>20.61</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A8" s="5"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -1812,8 +1834,9 @@
       <c r="V8" s="3"/>
       <c r="W8" s="3"/>
       <c r="X8" s="3"/>
-    </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="Y8" s="3"/>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>41</v>
       </c>
@@ -1872,8 +1895,9 @@
       </c>
       <c r="W9" s="12"/>
       <c r="X9" s="12"/>
-    </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="Y9" s="12"/>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>44</v>
       </c>
@@ -1932,8 +1956,9 @@
       </c>
       <c r="W10" s="12"/>
       <c r="X10" s="12"/>
-    </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="Y10" s="12"/>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>45</v>
       </c>
@@ -1960,23 +1985,24 @@
       <c r="V11" s="3"/>
       <c r="W11" s="3"/>
       <c r="X11" s="3"/>
-    </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="Y11" s="3"/>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
       <c r="C13" s="7" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
       <c r="C14" s="7" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
       <c r="C15" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
       <c r="C16" s="6" t="s">
         <v>48</v>
       </c>

</xml_diff>